<commit_message>
update comparison results and add the environment file
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Coding/bp/biorefineries/wwt/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A2B43E-958E-7E44-8778-68D8ACE011CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F94D8A0-CFF1-AA4D-AD20-C1216F51306D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11000" yWindow="6020" windowWidth="27400" windowHeight="18620" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
+    <workbookView xWindow="960" yWindow="10180" windowWidth="27400" windowHeight="18620" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="1" r:id="rId1"/>
@@ -631,7 +631,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,24 +737,24 @@
         <v>9</v>
       </c>
       <c r="C4" s="5">
-        <v>1.5335806045042899</v>
+        <v>1.5335806045303599</v>
       </c>
       <c r="D4" s="5">
-        <v>-12.794517510472099</v>
+        <v>-12.7945415905519</v>
       </c>
       <c r="E4" s="5">
-        <v>1.51205741348304</v>
+        <v>1.5120574133501901</v>
       </c>
       <c r="F4" s="5">
-        <v>-13.176638267636299</v>
+        <v>-13.1766382676365</v>
       </c>
       <c r="G4" s="10">
         <f t="shared" si="0"/>
-        <v>-1.4034600436412654E-2</v>
+        <v>-1.4034600539800832E-2</v>
       </c>
       <c r="H4" s="10">
         <f t="shared" si="1"/>
-        <v>2.9865976333335022E-2</v>
+        <v>2.9864038065010399E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -765,20 +765,20 @@
         <v>9</v>
       </c>
       <c r="C5" s="5">
-        <v>2.08890385830817</v>
+        <v>2.1288498018910502</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="5">
-        <v>2.0889122199132002</v>
+        <v>2.1292465237494902</v>
       </c>
       <c r="F5" s="5">
-        <v>0.196715214615172</v>
+        <v>0.72724579780821597</v>
       </c>
       <c r="G5" s="10">
         <f t="shared" si="0"/>
-        <v>4.0028673396781164E-6</v>
+        <v>1.8635502518193995E-4</v>
       </c>
       <c r="H5" s="10" t="str">
         <f t="shared" si="1"/>
@@ -793,24 +793,24 @@
         <v>9</v>
       </c>
       <c r="C6" s="5">
-        <v>2.3039218245397799</v>
+        <v>2.3535531988993199</v>
       </c>
       <c r="D6" s="5">
-        <v>1.3651391412168501</v>
+        <v>1.76992480536927</v>
       </c>
       <c r="E6" s="5">
-        <v>2.3039409165521398</v>
+        <v>2.3534974075271098</v>
       </c>
       <c r="F6" s="5">
-        <v>1.4340793082500201</v>
+        <v>1.8590999877697201</v>
       </c>
       <c r="G6" s="10">
         <f t="shared" si="0"/>
-        <v>8.2867448698084453E-6</v>
+        <v>-2.37051672493382E-5</v>
       </c>
       <c r="H6" s="10">
         <f t="shared" si="1"/>
-        <v>5.0500469110949721E-2</v>
+        <v>5.0383599421809859E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -821,24 +821,24 @@
         <v>9</v>
       </c>
       <c r="C7" s="5">
-        <v>1.9316247135882301</v>
+        <v>1.99972471216735</v>
       </c>
       <c r="D7" s="5">
-        <v>1.0044806875743699</v>
+        <v>1.2669205590255099</v>
       </c>
       <c r="E7" s="5">
-        <v>1.9363962935719301</v>
+        <v>1.9983229422348301</v>
       </c>
       <c r="F7" s="5">
-        <v>0.89072198708219796</v>
+        <v>1.49180522952494</v>
       </c>
       <c r="G7" s="10">
         <f t="shared" si="0"/>
-        <v>2.4702417349155986E-3</v>
+        <v>-7.0098145209231079E-4</v>
       </c>
       <c r="H7" s="10">
         <f t="shared" si="1"/>
-        <v>-0.1132512569921853</v>
+        <v>0.17750495001234085</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -849,24 +849,24 @@
         <v>11</v>
       </c>
       <c r="C8" s="6">
-        <v>1.39877834058841</v>
+        <v>1.4179202730054401</v>
       </c>
       <c r="D8" s="6">
-        <v>4.3970713685636396</v>
+        <v>4.4994033158573004</v>
       </c>
       <c r="E8" s="6">
-        <v>1.3752830264271001</v>
+        <v>1.3751680588605399</v>
       </c>
       <c r="F8" s="6">
-        <v>4.5058112500984802</v>
+        <v>4.5054514989784797</v>
       </c>
       <c r="G8" s="11">
         <f t="shared" si="0"/>
-        <v>-1.6797024574620137E-2</v>
+        <v>-3.0151352624560528E-2</v>
       </c>
       <c r="H8" s="11">
         <f t="shared" si="1"/>
-        <v>2.4730069726014454E-2</v>
+        <v>1.3442189322890219E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor updates to the formatting of the comparison spreadsheet
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Coding/bp/biorefineries/wwt/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F94D8A0-CFF1-AA4D-AD20-C1216F51306D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F243D9E8-2B15-0A43-A308-5F33EFA21C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="10180" windowWidth="27400" windowHeight="18620" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
+    <workbookView xWindow="16440" yWindow="8880" windowWidth="27400" windowHeight="18620" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>NA</t>
   </si>
@@ -120,12 +120,6 @@
     <t>MPSP_original</t>
   </si>
   <si>
-    <t>MPSP_diff</t>
-  </si>
-  <si>
-    <t>GWP_diff</t>
-  </si>
-  <si>
     <t>GWP_original</t>
   </si>
   <si>
@@ -133,6 +127,21 @@
   </si>
   <si>
     <t>GWP_wwt</t>
+  </si>
+  <si>
+    <t>MPSP_diff_rel</t>
+  </si>
+  <si>
+    <t>MPSP_diff_abs</t>
+  </si>
+  <si>
+    <t>GWP_diff_abs</t>
+  </si>
+  <si>
+    <t>GWP_diff_rel</t>
+  </si>
+  <si>
+    <t>consistency</t>
   </si>
 </sst>
 </file>
@@ -264,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -301,13 +310,162 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -628,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39242B9-9C3C-2E4F-A73C-DDCC8F0322B4}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,12 +800,15 @@
     <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -658,22 +819,34 @@
         <v>12</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>14</v>
+      <c r="I1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -692,16 +865,32 @@
       <c r="F2" s="5">
         <v>2.6959830621634202</v>
       </c>
-      <c r="G2" s="9">
-        <f t="shared" ref="G2:G8" si="0">(E2-C2)/C2</f>
+      <c r="G2" s="13">
+        <f>(E2-C2)</f>
+        <v>-2.5967294468890012E-2</v>
+      </c>
+      <c r="H2" s="9">
+        <f t="shared" ref="H2:H8" si="0">(E2-C2)/C2</f>
         <v>-1.7908787716264082E-2</v>
       </c>
-      <c r="H2" s="9" t="str">
-        <f t="shared" ref="H2:H8" si="1">IF(D2&lt;&gt;"NA",(F2-D2)/D2, "NA")</f>
-        <v>NA</v>
+      <c r="I2" s="9" t="b">
+        <f>IF(AND(ABS(G2)&gt;0.1, ABS(H2)&gt;0.1), FALSE, TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="13">
+        <f>IF(D2&lt;&gt;"NA",(F2-D2), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="9">
+        <f>IF(D2&lt;&gt;"NA",(F2-D2)/D2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="9" t="b">
+        <f>IF(AND(ABS(J2)&gt;0.1, ABS(K2)&gt;0.1), FALSE, TRUE)</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -720,16 +909,32 @@
       <c r="F3" s="5">
         <v>-1.5833219514494701</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="14">
+        <f t="shared" ref="G3:G8" si="1">(E3-C3)</f>
+        <v>-7.2091432111200948E-3</v>
+      </c>
+      <c r="H3" s="10">
         <f t="shared" si="0"/>
         <v>-3.6396459024420958E-3</v>
       </c>
-      <c r="H3" s="10">
-        <f t="shared" si="1"/>
+      <c r="I3" s="10" t="b">
+        <f t="shared" ref="I3:I8" si="2">IF(AND(ABS(G3)&gt;0.1, ABS(H3)&gt;0.1), FALSE, TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="14">
+        <f>IF(D3&lt;&gt;"NA",(F3-D3), 0)</f>
+        <v>-8.0731348481330123E-2</v>
+      </c>
+      <c r="K3" s="10">
+        <f t="shared" ref="K3:K8" si="3">IF(D3&lt;&gt;"NA",(F3-D3)/D3, 0)</f>
         <v>5.3728106858819416E-2</v>
       </c>
+      <c r="L3" s="10" t="b">
+        <f t="shared" ref="L3:L8" si="4">IF(AND(ABS(J3)&gt;0.1, ABS(K3)&gt;0.1), FALSE, TRUE)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -748,16 +953,32 @@
       <c r="F4" s="5">
         <v>-13.1766382676365</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="14">
+        <f t="shared" si="1"/>
+        <v>-2.1523191180169876E-2</v>
+      </c>
+      <c r="H4" s="10">
         <f t="shared" si="0"/>
         <v>-1.4034600539800832E-2</v>
       </c>
-      <c r="H4" s="10">
-        <f t="shared" si="1"/>
+      <c r="I4" s="10" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="14">
+        <f>IF(D4&lt;&gt;"NA",(F4-D4), 0)</f>
+        <v>-0.3820966770846006</v>
+      </c>
+      <c r="K4" s="10">
+        <f t="shared" si="3"/>
         <v>2.9864038065010399E-2</v>
       </c>
+      <c r="L4" s="10" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -776,16 +997,32 @@
       <c r="F5" s="5">
         <v>0.72724579780821597</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="14">
+        <f t="shared" si="1"/>
+        <v>3.9672185843997454E-4</v>
+      </c>
+      <c r="H5" s="10">
         <f t="shared" si="0"/>
         <v>1.8635502518193995E-4</v>
       </c>
-      <c r="H5" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
+      <c r="I5" s="10" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
+        <f>IF(D5&lt;&gt;"NA",(F5-D5), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="10" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -804,16 +1041,32 @@
       <c r="F6" s="5">
         <v>1.8590999877697201</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="14">
+        <f t="shared" si="1"/>
+        <v>-5.5791372210123313E-5</v>
+      </c>
+      <c r="H6" s="10">
         <f t="shared" si="0"/>
         <v>-2.37051672493382E-5</v>
       </c>
-      <c r="H6" s="10">
-        <f t="shared" si="1"/>
+      <c r="I6" s="10" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J6" s="14">
+        <f>IF(D6&lt;&gt;"NA",(F6-D6), 0)</f>
+        <v>8.9175182400450081E-2</v>
+      </c>
+      <c r="K6" s="10">
+        <f t="shared" si="3"/>
         <v>5.0383599421809859E-2</v>
       </c>
+      <c r="L6" s="10" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -832,16 +1085,32 @@
       <c r="F7" s="5">
         <v>1.49180522952494</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="14">
+        <f t="shared" si="1"/>
+        <v>-1.4017699325199473E-3</v>
+      </c>
+      <c r="H7" s="10">
         <f t="shared" si="0"/>
         <v>-7.0098145209231079E-4</v>
       </c>
-      <c r="H7" s="10">
-        <f t="shared" si="1"/>
+      <c r="I7" s="10" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="14">
+        <f>IF(D7&lt;&gt;"NA",(F7-D7), 0)</f>
+        <v>0.22488467049943006</v>
+      </c>
+      <c r="K7" s="10">
+        <f t="shared" si="3"/>
         <v>0.17750495001234085</v>
       </c>
+      <c r="L7" s="10" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -860,18 +1129,54 @@
       <c r="F8" s="6">
         <v>4.5054514989784797</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="15">
+        <f t="shared" si="1"/>
+        <v>-4.2752214144900158E-2</v>
+      </c>
+      <c r="H8" s="11">
         <f t="shared" si="0"/>
         <v>-3.0151352624560528E-2</v>
       </c>
-      <c r="H8" s="11">
-        <f t="shared" si="1"/>
+      <c r="I8" s="11" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="15">
+        <f>IF(D8&lt;&gt;"NA",(F8-D8), 0)</f>
+        <v>6.0481831211793846E-3</v>
+      </c>
+      <c r="K8" s="11">
+        <f t="shared" si="3"/>
         <v>1.3442189322890219E-3</v>
+      </c>
+      <c r="L8" s="11" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:H8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
+  <conditionalFormatting sqref="L2:L8 H2:I8">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G8">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="notBetween">
+      <formula>-0.1</formula>
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J8">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="notBetween">
+      <formula>-0.1</formula>
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K8">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="notBetween">
       <formula>-0.1</formula>
       <formula>0.1</formula>
     </cfRule>

</xml_diff>

<commit_message>
update comparison spreadsheet with updates in the cornstover biorefinery
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Coding/bp/biorefineries/wwt/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AAA617-BB61-5246-96E8-7ACF0411D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1735A3-E27A-9E41-A81B-2CF965BA0AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="10420" windowWidth="27400" windowHeight="18620" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
+    <workbookView xWindow="1040" yWindow="2980" windowWidth="27400" windowHeight="18620" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="1" r:id="rId1"/>
@@ -695,7 +695,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,7 +927,7 @@
         <v>2.1292465237494902</v>
       </c>
       <c r="F5" s="5">
-        <v>0.72724579780821597</v>
+        <v>0.87251355781668705</v>
       </c>
       <c r="G5" s="5">
         <v>1.96345339780636</v>

</xml_diff>

<commit_message>
update with newer biosteam/biorefinery modules
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Coding/bp/biorefineries/wwt/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1735A3-E27A-9E41-A81B-2CF965BA0AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588FDC83-26E2-EE4E-9D71-46393A46A43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="2980" windowWidth="27400" windowHeight="18620" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
+    <workbookView xWindow="4280" yWindow="2720" windowWidth="27400" windowHeight="15920" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>Yalin Li</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{86C80020-94DF-A34D-9769-E78F95407B34}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{332F555C-9942-7143-8DF9-AF9B87281018}">
       <text>
         <r>
           <rPr>
@@ -279,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -290,13 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -324,6 +318,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -331,7 +346,57 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -695,7 +760,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,46 +782,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -767,45 +832,45 @@
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1.449975</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5">
-        <v>1.42400770553111</v>
-      </c>
-      <c r="F2" s="5">
-        <v>2.6959830621634202</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1.44619981691902</v>
-      </c>
-      <c r="H2" s="5">
-        <v>2.6441211717736399</v>
-      </c>
-      <c r="I2" s="13">
+      <c r="E2" s="4">
+        <v>1.4245895770530499</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2.6959830587204801</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1.44065126995148</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2.5803373928586102</v>
+      </c>
+      <c r="I2" s="11">
         <f>(E2-C2)</f>
-        <v>-2.5967294468890012E-2</v>
-      </c>
-      <c r="J2" s="9">
+        <v>-2.538542294695012E-2</v>
+      </c>
+      <c r="J2" s="7">
         <f t="shared" ref="J2:J8" si="0">(E2-C2)/C2</f>
-        <v>-1.7908787716264082E-2</v>
-      </c>
-      <c r="K2" s="9" t="b">
+        <v>-1.7507490092553403E-2</v>
+      </c>
+      <c r="K2" s="7" t="b">
         <f>IF(AND(ABS(I2)&gt;0.1, ABS(J2)&gt;0.1), FALSE, TRUE)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="11">
         <f t="shared" ref="L2:L8" si="1">IF(D2&lt;&gt;"NA",(F2-D2), 0)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="7">
         <f>IF(D2&lt;&gt;"NA",(F2-D2)/D2, 0)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="9" t="b">
+      <c r="N2" s="7" t="b">
         <f>IF(AND(ABS(L2)&gt;0.1, ABS(M2)&gt;0.1), FALSE, TRUE)</f>
         <v>1</v>
       </c>
@@ -817,45 +882,45 @@
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5">
-        <v>1.98072653339243</v>
-      </c>
-      <c r="D3" s="5">
-        <v>-1.50259060296814</v>
-      </c>
-      <c r="E3" s="5">
-        <v>1.9735173901813099</v>
-      </c>
-      <c r="F3" s="5">
-        <v>-1.5833219514494701</v>
-      </c>
-      <c r="G3" s="5">
-        <v>2.0207467422379302</v>
-      </c>
-      <c r="H3" s="5">
-        <v>-1.7700895212399199</v>
+      <c r="C3" s="4">
+        <v>2.0069969392743201</v>
+      </c>
+      <c r="D3" s="4">
+        <v>-1.49834624704022</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.99400148127827</v>
+      </c>
+      <c r="F3" s="4">
+        <v>-1.5789338598814799</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2.02343360509968</v>
+      </c>
+      <c r="H3" s="4">
+        <v>-1.93520940173647</v>
       </c>
       <c r="I3" s="14">
         <f t="shared" ref="I3:I8" si="2">(E3-C3)</f>
-        <v>-7.2091432111200948E-3</v>
-      </c>
-      <c r="J3" s="10">
+        <v>-1.2995457996050064E-2</v>
+      </c>
+      <c r="J3" s="15">
         <f t="shared" si="0"/>
-        <v>-3.6396459024420958E-3</v>
-      </c>
-      <c r="K3" s="10" t="b">
+        <v>-6.4750761407483242E-3</v>
+      </c>
+      <c r="K3" s="8" t="b">
         <f t="shared" ref="K3:K8" si="3">IF(AND(ABS(I3)&gt;0.1, ABS(J3)&gt;0.1), FALSE, TRUE)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="12">
         <f t="shared" si="1"/>
-        <v>-8.0731348481330123E-2</v>
-      </c>
-      <c r="M3" s="10">
+        <v>-8.0587612841259926E-2</v>
+      </c>
+      <c r="M3" s="8">
         <f t="shared" ref="M3:M8" si="4">IF(D3&lt;&gt;"NA",(F3-D3)/D3, 0)</f>
-        <v>5.3728106858819416E-2</v>
-      </c>
-      <c r="N3" s="10" t="b">
+        <v>5.3784372604429607E-2</v>
+      </c>
+      <c r="N3" s="8" t="b">
         <f t="shared" ref="N3:N8" si="5">IF(AND(ABS(L3)&gt;0.1, ABS(M3)&gt;0.1), FALSE, TRUE)</f>
         <v>1</v>
       </c>
@@ -867,45 +932,45 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5">
-        <v>1.5335806045303599</v>
-      </c>
-      <c r="D4" s="5">
-        <v>-12.7945415905519</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1.5120574133501901</v>
-      </c>
-      <c r="F4" s="5">
-        <v>-13.1766382676365</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1.6392340672605901</v>
-      </c>
-      <c r="H4" s="5">
-        <v>-13.3946003253452</v>
+      <c r="C4" s="20">
+        <v>1.62033891808155</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-13.0790883729995</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.5984241061734099</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-13.418638499597799</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1.70276209508825</v>
+      </c>
+      <c r="H4" s="4">
+        <v>-14.065598314481599</v>
       </c>
       <c r="I4" s="14">
         <f t="shared" si="2"/>
-        <v>-2.1523191180169876E-2</v>
-      </c>
-      <c r="J4" s="10">
+        <v>-2.1914811908140042E-2</v>
+      </c>
+      <c r="J4" s="15">
         <f t="shared" si="0"/>
-        <v>-1.4034600539800832E-2</v>
-      </c>
-      <c r="K4" s="10" t="b">
+        <v>-1.3524832159241572E-2</v>
+      </c>
+      <c r="K4" s="8" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="12">
         <f t="shared" si="1"/>
-        <v>-0.3820966770846006</v>
-      </c>
-      <c r="M4" s="10">
+        <v>-0.33955012659829897</v>
+      </c>
+      <c r="M4" s="8">
         <f t="shared" si="4"/>
-        <v>2.9864038065010399E-2</v>
-      </c>
-      <c r="N4" s="10" t="b">
+        <v>2.5961299206393239E-2</v>
+      </c>
+      <c r="N4" s="8" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -917,45 +982,45 @@
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5">
-        <v>2.1288498018910502</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4">
+        <v>2.2043606950162902</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
-        <v>2.1292465237494902</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.87251355781668705</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1.96345339780636</v>
-      </c>
-      <c r="H5" s="5">
-        <v>-0.30890062078379998</v>
+      <c r="E5" s="4">
+        <v>2.2047743971404299</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.42090001234551</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1.77521719675212</v>
+      </c>
+      <c r="H5" s="4">
+        <v>-2.3757211244144001</v>
       </c>
       <c r="I5" s="14">
         <f t="shared" si="2"/>
-        <v>3.9672185843997454E-4</v>
-      </c>
-      <c r="J5" s="10">
+        <v>4.137021241397143E-4</v>
+      </c>
+      <c r="J5" s="15">
         <f t="shared" si="0"/>
-        <v>1.8635502518193995E-4</v>
-      </c>
-      <c r="K5" s="10" t="b">
+        <v>1.8767442418794218E-4</v>
+      </c>
+      <c r="K5" s="8" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N5" s="10" t="b">
+      <c r="N5" s="8" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -967,45 +1032,45 @@
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5">
-        <v>2.3535531988993199</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1.76992480536927</v>
-      </c>
-      <c r="E6" s="5">
-        <v>2.3534974075271098</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1.8590999877697201</v>
-      </c>
-      <c r="G6" s="5">
-        <v>2.1099166755697598</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1.1273919300223101</v>
+      <c r="C6" s="4">
+        <v>2.6284154714118699</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.82286666134993</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.6286053641353702</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.90308498431082</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2.29742812831527</v>
+      </c>
+      <c r="H6" s="4">
+        <v>-0.33666773212129097</v>
       </c>
       <c r="I6" s="14">
         <f t="shared" si="2"/>
-        <v>-5.5791372210123313E-5</v>
-      </c>
-      <c r="J6" s="10">
+        <v>1.8989272350022901E-4</v>
+      </c>
+      <c r="J6" s="15">
         <f t="shared" si="0"/>
-        <v>-2.37051672493382E-5</v>
-      </c>
-      <c r="K6" s="10" t="b">
+        <v>7.224608345431285E-5</v>
+      </c>
+      <c r="K6" s="8" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="12">
         <f t="shared" si="1"/>
-        <v>8.9175182400450081E-2</v>
-      </c>
-      <c r="M6" s="10">
+        <v>8.0218322960889932E-2</v>
+      </c>
+      <c r="M6" s="8">
         <f t="shared" si="4"/>
-        <v>5.0383599421809859E-2</v>
-      </c>
-      <c r="N6" s="10" t="b">
+        <v>4.4006687193172966E-2</v>
+      </c>
+      <c r="N6" s="8" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -1017,95 +1082,95 @@
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5">
-        <v>1.9996562891243299</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1.4157372841731599</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1.9983229422348301</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1.49180522952494</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1.7523427986257001</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.68677879509477802</v>
+      <c r="C7" s="4">
+        <v>2.7627905628818201</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.5614357145042701</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2.76279719460446</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.6156982112587499</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2.4922967876054898</v>
+      </c>
+      <c r="H7" s="4">
+        <v>-0.86378104562301405</v>
       </c>
       <c r="I7" s="14">
         <f t="shared" si="2"/>
-        <v>-1.3333468894998202E-3</v>
-      </c>
-      <c r="J7" s="10">
+        <v>6.6317226399270623E-6</v>
+      </c>
+      <c r="J7" s="15">
         <f t="shared" si="0"/>
-        <v>-6.6678803589976284E-4</v>
-      </c>
-      <c r="K7" s="10" t="b">
+        <v>2.4003711063098552E-6</v>
+      </c>
+      <c r="K7" s="8" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="12">
         <f t="shared" si="1"/>
-        <v>7.6067945351780075E-2</v>
-      </c>
-      <c r="M7" s="10">
+        <v>5.4262496754479805E-2</v>
+      </c>
+      <c r="M7" s="8">
         <f t="shared" si="4"/>
-        <v>5.3730269169400602E-2</v>
-      </c>
-      <c r="N7" s="10" t="b">
+        <v>3.4751668768961935E-2</v>
+      </c>
+      <c r="N7" s="8" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6">
-        <v>1.4179202730054401</v>
-      </c>
-      <c r="D8" s="6">
-        <v>4.4994033158573004</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1.3751680588605399</v>
-      </c>
-      <c r="F8" s="6">
-        <v>4.5054514989784797</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1.3029467468828</v>
-      </c>
-      <c r="H8" s="6">
-        <v>4.2002867619759003</v>
-      </c>
-      <c r="I8" s="15">
+      <c r="C8" s="17">
+        <v>1.43328539923927</v>
+      </c>
+      <c r="D8" s="17">
+        <v>4.6067986222162496</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1.3905358154549301</v>
+      </c>
+      <c r="F8" s="17">
+        <v>4.6038332682662597</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1.27394079067161</v>
+      </c>
+      <c r="H8" s="17">
+        <v>3.3845987314102701</v>
+      </c>
+      <c r="I8" s="18">
         <f t="shared" si="2"/>
-        <v>-4.2752214144900158E-2</v>
-      </c>
-      <c r="J8" s="11">
+        <v>-4.2749583784339906E-2</v>
+      </c>
+      <c r="J8" s="19">
         <f t="shared" si="0"/>
-        <v>-3.0151352624560528E-2</v>
-      </c>
-      <c r="K8" s="11" t="b">
+        <v>-2.9826288474737592E-2</v>
+      </c>
+      <c r="K8" s="9" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="13">
         <f t="shared" si="1"/>
-        <v>6.0481831211793846E-3</v>
-      </c>
-      <c r="M8" s="11">
+        <v>-2.9653539499898685E-3</v>
+      </c>
+      <c r="M8" s="9">
         <f t="shared" si="4"/>
-        <v>1.3442189322890219E-3</v>
-      </c>
-      <c r="N8" s="11" t="b">
+        <v>-6.4369081289758847E-4</v>
+      </c>
+      <c r="N8" s="9" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
update baseline comparison results
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Coding/bp/biorefineries/wwt/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588FDC83-26E2-EE4E-9D71-46393A46A43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68995569-F608-974A-A55F-E958F8825670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2720" windowWidth="27400" windowHeight="15920" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
+    <workbookView xWindow="3060" yWindow="4900" windowWidth="27840" windowHeight="19660" xr2:uid="{781C18B9-31A8-C44F-AD55-75724E8108D5}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="1" r:id="rId1"/>
@@ -79,10 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
-  <si>
-    <t>NA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>corn</t>
   </si>
@@ -148,6 +145,18 @@
   </si>
   <si>
     <t>GWP_new</t>
+  </si>
+  <si>
+    <t>MPSP_RIN</t>
+  </si>
+  <si>
+    <t>GWP_RIN</t>
+  </si>
+  <si>
+    <t>MPSP_no WWT</t>
+  </si>
+  <si>
+    <t>GWP_no WWT</t>
   </si>
 </sst>
 </file>
@@ -279,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -338,65 +347,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -458,6 +414,1909 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>cn</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$C$1,comparison!$E$1,comparison!$G$1,comparison!$I$1,comparison!$K$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>MPSP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPSP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPSP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPSP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPSP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$C$2,comparison!$E$2,comparison!$G$2,comparison!$I$2,comparison!$K$2)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.449975</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4245895770530499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.44065126995148</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.39536681050294</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4248677101382301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-0F33-BF48-9EB2-3CB6B9E5499E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>sc1g</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$C$1,comparison!$E$1,comparison!$G$1,comparison!$I$1,comparison!$K$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>MPSP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPSP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPSP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPSP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPSP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$C$3,comparison!$E$3,comparison!$G$3,comparison!$I$3,comparison!$K$3)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0069969392743201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.99400148127827</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.02343360509968</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.96899499440812</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9924452139376101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-0F33-BF48-9EB2-3CB6B9E5499E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>oc1g</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$C$1,comparison!$E$1,comparison!$G$1,comparison!$I$1,comparison!$K$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>MPSP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPSP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPSP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPSP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPSP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$C$4,comparison!$E$4,comparison!$G$4,comparison!$I$4,comparison!$K$4)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.6203389181338299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.59842410614715</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.70276209508825</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6362717538184399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6017675297771401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0F33-BF48-9EB2-3CB6B9E5499E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>cs</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$C$1,comparison!$E$1,comparison!$G$1,comparison!$I$1,comparison!$K$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>MPSP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPSP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPSP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPSP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPSP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$C$5,comparison!$E$5,comparison!$G$5,comparison!$I$5,comparison!$K$5)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.2043606950162902</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2047743971935598</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.77521719675212</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84718608745318502</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1736676495168399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-0F33-BF48-9EB2-3CB6B9E5499E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>sc2g</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$C$1,comparison!$E$1,comparison!$G$1,comparison!$I$1,comparison!$K$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>MPSP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPSP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPSP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPSP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPSP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$C$6,comparison!$E$6,comparison!$G$6,comparison!$I$6,comparison!$K$6)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.6284154714118699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6286053641637701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2974281283806999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9897717794471701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2811675063762298</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-0F33-BF48-9EB2-3CB6B9E5499E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>oc2g</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$C$1,comparison!$E$1,comparison!$G$1,comparison!$I$1,comparison!$K$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>MPSP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPSP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPSP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPSP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPSP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$C$7,comparison!$E$7,comparison!$G$7,comparison!$I$7,comparison!$K$7)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.76279056279497</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7627971946497198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4922967876054898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0246959464105001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5290595300179999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-0F33-BF48-9EB2-3CB6B9E5499E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>la</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$C$8,comparison!$E$8,comparison!$G$8,comparison!$I$8,comparison!$K$8)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.43328539923927</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3905358154549301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.27394079066307</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84987047152756601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3691704716730699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-0F33-BF48-9EB2-3CB6B9E5499E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="601792111"/>
+        <c:axId val="601793759"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="601792111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601793759"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="601793759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601792111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>cn</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$2,comparison!$F$2,comparison!$H$2,comparison!$J$2,comparison!$L$2)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>2.6959830587204801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5803373928586102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.56810572110839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6975301418335702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F49-8943-BE1D-4EA7F193C06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>sc1g</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$3,comparison!$F$3,comparison!$H$3,comparison!$J$3,comparison!$L$3)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-1.49834624704022</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.5789338598814799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.93520940173647</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.7825729884558801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.5857074658830499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8F49-8943-BE1D-4EA7F193C06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>oc1g</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$4,comparison!$F$4,comparison!$H$4,comparison!$J$4,comparison!$L$4)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-13.0790883729995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-13.418638499597799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14.065598314481599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-13.862100570089201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-13.621031724160501</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8F49-8943-BE1D-4EA7F193C06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>cs</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$5,comparison!$F$5,comparison!$H$5,comparison!$J$5,comparison!$L$5)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>1.42090001234551</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.3757211244144001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.79650894315835297</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0432172616145299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8F49-8943-BE1D-4EA7F193C06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>sc2g</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$6,comparison!$F$6,comparison!$H$6,comparison!$J$6,comparison!$L$6)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.82286666134993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.90308498431082</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.33666773212129097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19153136343829799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2678302360120199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8F49-8943-BE1D-4EA7F193C06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>oc2g</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$7,comparison!$F$7,comparison!$H$7,comparison!$J$7,comparison!$L$7)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.56143559768429</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6156982112596601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.86378104562301306</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-9.8444064306308005E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4573303246492699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8F49-8943-BE1D-4EA7F193C06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>la</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$8,comparison!$F$8,comparison!$H$8,comparison!$J$8,comparison!$L$8)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6067986222162496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6038332682662597</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3845987314102701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9127558368689099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0701466343454697</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-8F49-8943-BE1D-4EA7F193C06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="601792111"/>
+        <c:axId val="601793759"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="601792111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601793759"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="601793759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="-3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601792111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>cn</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-FEFA-1C41-BE0D-45EB5C86D064}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$2,comparison!$F$2,comparison!$H$2,comparison!$J$2,comparison!$L$2)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>2.6959830587204801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5803373928586102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.56810572110839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6975301418335702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FEFA-1C41-BE0D-45EB5C86D064}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>sc1g</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$3,comparison!$F$3,comparison!$H$3,comparison!$J$3,comparison!$L$3)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-1.49834624704022</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.5789338598814799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.93520940173647</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.7825729884558801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.5857074658830499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FEFA-1C41-BE0D-45EB5C86D064}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>oc1g</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$4,comparison!$F$4,comparison!$H$4,comparison!$J$4,comparison!$L$4)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-13.0790883729995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-13.418638499597799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14.065598314481599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-13.862100570089201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-13.621031724160501</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FEFA-1C41-BE0D-45EB5C86D064}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>cs</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$5,comparison!$F$5,comparison!$H$5,comparison!$J$5,comparison!$L$5)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>1.42090001234551</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.3757211244144001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.79650894315835297</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0432172616145299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FEFA-1C41-BE0D-45EB5C86D064}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>sc2g</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$6,comparison!$F$6,comparison!$H$6,comparison!$J$6,comparison!$L$6)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.82286666134993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.90308498431082</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.33666773212129097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19153136343829799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2678302360120199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-FEFA-1C41-BE0D-45EB5C86D064}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>oc2g</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$7,comparison!$F$7,comparison!$H$7,comparison!$J$7,comparison!$L$7)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.56143559768429</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6156982112596601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.86378104562301306</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-9.8444064306308005E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4573303246492699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-FEFA-1C41-BE0D-45EB5C86D064}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>la</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(comparison!$D$1,comparison!$F$1,comparison!$H$1,comparison!$J$1,comparison!$L$1)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GWP_original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWP_exist</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GWP_new</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GWP_RIN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GWP_no WWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(comparison!$D$8,comparison!$F$8,comparison!$H$8,comparison!$J$8,comparison!$L$8)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6067986222162496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6038332682662597</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3845987314102701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9127558368689099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0701466343454697</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-FEFA-1C41-BE0D-45EB5C86D064}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="601792111"/>
+        <c:axId val="601793759"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="601792111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601793759"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="601793759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="-10"/>
+          <c:min val="-15"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601792111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>536866</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>204354</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681183</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCD3C701-CEC1-3B85-9F0B-70066D6A3BC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>554182</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>184728</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>63499</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>84283</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{995400E6-5EFB-1442-B3AC-B54AEF2BF5DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>790862</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>107374</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A37873-E75A-A74D-9652-022D700071C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -757,10 +2616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39242B9-9C3C-2E4F-A73C-DDCC8F0322B4}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,71 +2632,84 @@
     <col min="6" max="6" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="4">
         <v>1.449975</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="D2" s="4"/>
       <c r="E2" s="4">
         <v>1.4245895770530499</v>
       </c>
@@ -850,37 +2722,49 @@
       <c r="H2" s="4">
         <v>2.5803373928586102</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="4">
+        <v>1.39536681050294</v>
+      </c>
+      <c r="J2" s="4">
+        <v>2.56810572110839</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1.4248677101382301</v>
+      </c>
+      <c r="L2" s="4">
+        <v>2.6975301418335702</v>
+      </c>
+      <c r="M2" s="11">
         <f>(E2-C2)</f>
         <v>-2.538542294695012E-2</v>
       </c>
-      <c r="J2" s="7">
-        <f t="shared" ref="J2:J8" si="0">(E2-C2)/C2</f>
+      <c r="N2" s="7">
+        <f t="shared" ref="N2:N8" si="0">(E2-C2)/C2</f>
         <v>-1.7507490092553403E-2</v>
       </c>
-      <c r="K2" s="7" t="b">
-        <f>IF(AND(ABS(I2)&gt;0.1, ABS(J2)&gt;0.1), FALSE, TRUE)</f>
+      <c r="O2" s="7" t="b">
+        <f>IF(AND(ABS(M2)&gt;0.1, ABS(N2)&gt;0.1), FALSE, TRUE)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="11">
-        <f t="shared" ref="L2:L8" si="1">IF(D2&lt;&gt;"NA",(F2-D2), 0)</f>
+      <c r="P2" s="11">
+        <f>IF(D2&lt;&gt;"",(F2-D2), 0)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="7">
-        <f>IF(D2&lt;&gt;"NA",(F2-D2)/D2, 0)</f>
+      <c r="Q2" s="7">
+        <f>IF(D2&lt;&gt;"",(F2-D2)/D2, 0)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="7" t="b">
-        <f>IF(AND(ABS(L2)&gt;0.1, ABS(M2)&gt;0.1), FALSE, TRUE)</f>
+      <c r="R2" s="7" t="b">
+        <f>IF(AND(ABS(P2)&gt;0.1, ABS(Q2)&gt;0.1), FALSE, TRUE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4">
         <v>2.0069969392743201</v>
@@ -900,46 +2784,58 @@
       <c r="H3" s="4">
         <v>-1.93520940173647</v>
       </c>
-      <c r="I3" s="14">
-        <f t="shared" ref="I3:I8" si="2">(E3-C3)</f>
+      <c r="I3" s="4">
+        <v>1.96899499440812</v>
+      </c>
+      <c r="J3" s="4">
+        <v>-1.7825729884558801</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1.9924452139376101</v>
+      </c>
+      <c r="L3" s="4">
+        <v>-1.5857074658830499</v>
+      </c>
+      <c r="M3" s="14">
+        <f t="shared" ref="M3:M8" si="1">(E3-C3)</f>
         <v>-1.2995457996050064E-2</v>
       </c>
-      <c r="J3" s="15">
+      <c r="N3" s="15">
         <f t="shared" si="0"/>
         <v>-6.4750761407483242E-3</v>
       </c>
-      <c r="K3" s="8" t="b">
-        <f t="shared" ref="K3:K8" si="3">IF(AND(ABS(I3)&gt;0.1, ABS(J3)&gt;0.1), FALSE, TRUE)</f>
+      <c r="O3" s="8" t="b">
+        <f t="shared" ref="O3:O8" si="2">IF(AND(ABS(M3)&gt;0.1, ABS(N3)&gt;0.1), FALSE, TRUE)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="12">
-        <f t="shared" si="1"/>
+      <c r="P3" s="12">
+        <f t="shared" ref="P3:P8" si="3">IF(D3&lt;&gt;"",(F3-D3), 0)</f>
         <v>-8.0587612841259926E-2</v>
       </c>
-      <c r="M3" s="8">
-        <f t="shared" ref="M3:M8" si="4">IF(D3&lt;&gt;"NA",(F3-D3)/D3, 0)</f>
+      <c r="Q3" s="8">
+        <f t="shared" ref="Q3:Q8" si="4">IF(D3&lt;&gt;"",(F3-D3)/D3, 0)</f>
         <v>5.3784372604429607E-2</v>
       </c>
-      <c r="N3" s="8" t="b">
-        <f t="shared" ref="N3:N8" si="5">IF(AND(ABS(L3)&gt;0.1, ABS(M3)&gt;0.1), FALSE, TRUE)</f>
+      <c r="R3" s="8" t="b">
+        <f t="shared" ref="R3:R8" si="5">IF(AND(ABS(P3)&gt;0.1, ABS(Q3)&gt;0.1), FALSE, TRUE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="20">
-        <v>1.62033891808155</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.6203389181338299</v>
       </c>
       <c r="D4" s="4">
         <v>-13.0790883729995</v>
       </c>
       <c r="E4" s="4">
-        <v>1.5984241061734099</v>
+        <v>1.59842410614715</v>
       </c>
       <c r="F4" s="4">
         <v>-13.418638499597799</v>
@@ -950,46 +2846,56 @@
       <c r="H4" s="4">
         <v>-14.065598314481599</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="4">
+        <v>1.6362717538184399</v>
+      </c>
+      <c r="J4" s="4">
+        <v>-13.862100570089201</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.6017675297771401</v>
+      </c>
+      <c r="L4" s="4">
+        <v>-13.621031724160501</v>
+      </c>
+      <c r="M4" s="14">
+        <f t="shared" si="1"/>
+        <v>-2.1914811986679883E-2</v>
+      </c>
+      <c r="N4" s="15">
+        <f t="shared" si="0"/>
+        <v>-1.3524832207276438E-2</v>
+      </c>
+      <c r="O4" s="8" t="b">
         <f t="shared" si="2"/>
-        <v>-2.1914811908140042E-2</v>
-      </c>
-      <c r="J4" s="15">
-        <f t="shared" si="0"/>
-        <v>-1.3524832159241572E-2</v>
-      </c>
-      <c r="K4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" s="12">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L4" s="12">
-        <f t="shared" si="1"/>
         <v>-0.33955012659829897</v>
       </c>
-      <c r="M4" s="8">
+      <c r="Q4" s="8">
         <f t="shared" si="4"/>
         <v>2.5961299206393239E-2</v>
       </c>
-      <c r="N4" s="8" t="b">
+      <c r="R4" s="8" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="4">
         <v>2.2043606950162902</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="4">
-        <v>2.2047743971404299</v>
+        <v>2.2047743971935598</v>
       </c>
       <c r="F5" s="4">
         <v>1.42090001234551</v>
@@ -1000,37 +2906,49 @@
       <c r="H5" s="4">
         <v>-2.3757211244144001</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="4">
+        <v>0.84718608745318502</v>
+      </c>
+      <c r="J5" s="4">
+        <v>-0.79650894315835297</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2.1736676495168399</v>
+      </c>
+      <c r="L5" s="4">
+        <v>3.0432172616145299</v>
+      </c>
+      <c r="M5" s="14">
+        <f t="shared" si="1"/>
+        <v>4.1370217726965919E-4</v>
+      </c>
+      <c r="N5" s="15">
+        <f t="shared" si="0"/>
+        <v>1.8767444829014335E-4</v>
+      </c>
+      <c r="O5" s="8" t="b">
         <f t="shared" si="2"/>
-        <v>4.137021241397143E-4</v>
-      </c>
-      <c r="J5" s="15">
-        <f t="shared" si="0"/>
-        <v>1.8767442418794218E-4</v>
-      </c>
-      <c r="K5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" s="12">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L5" s="12">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M5" s="8">
+      <c r="Q5" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N5" s="8" t="b">
+      <c r="R5" s="8" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4">
         <v>2.6284154714118699</v>
@@ -1039,98 +2957,122 @@
         <v>1.82286666134993</v>
       </c>
       <c r="E6" s="4">
-        <v>2.6286053641353702</v>
+        <v>2.6286053641637701</v>
       </c>
       <c r="F6" s="4">
         <v>1.90308498431082</v>
       </c>
       <c r="G6" s="4">
-        <v>2.29742812831527</v>
+        <v>2.2974281283806999</v>
       </c>
       <c r="H6" s="4">
         <v>-0.33666773212129097</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="4">
+        <v>1.9897717794471701</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.19153136343829799</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2.2811675063762298</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.2678302360120199</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" si="1"/>
+        <v>1.8989275190017807E-4</v>
+      </c>
+      <c r="N6" s="15">
+        <f t="shared" si="0"/>
+        <v>7.2246094259282372E-5</v>
+      </c>
+      <c r="O6" s="8" t="b">
         <f t="shared" si="2"/>
-        <v>1.8989272350022901E-4</v>
-      </c>
-      <c r="J6" s="15">
-        <f t="shared" si="0"/>
-        <v>7.224608345431285E-5</v>
-      </c>
-      <c r="K6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="12">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L6" s="12">
-        <f t="shared" si="1"/>
         <v>8.0218322960889932E-2</v>
       </c>
-      <c r="M6" s="8">
+      <c r="Q6" s="8">
         <f t="shared" si="4"/>
         <v>4.4006687193172966E-2</v>
       </c>
-      <c r="N6" s="8" t="b">
+      <c r="R6" s="8" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>2.7627905628818201</v>
+        <v>2.76279056279497</v>
       </c>
       <c r="D7" s="4">
-        <v>1.5614357145042701</v>
+        <v>1.56143559768429</v>
       </c>
       <c r="E7" s="4">
-        <v>2.76279719460446</v>
+        <v>2.7627971946497198</v>
       </c>
       <c r="F7" s="4">
-        <v>1.6156982112587499</v>
+        <v>1.6156982112596601</v>
       </c>
       <c r="G7" s="4">
         <v>2.4922967876054898</v>
       </c>
       <c r="H7" s="4">
-        <v>-0.86378104562301405</v>
-      </c>
-      <c r="I7" s="14">
+        <v>-0.86378104562301306</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2.0246959464105001</v>
+      </c>
+      <c r="J7" s="4">
+        <v>-9.8444064306308005E-2</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2.5290595300179999</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1.4573303246492699</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="1"/>
+        <v>6.6318547498056546E-6</v>
+      </c>
+      <c r="N7" s="15">
+        <f t="shared" si="0"/>
+        <v>2.4004189239362955E-6</v>
+      </c>
+      <c r="O7" s="8" t="b">
         <f t="shared" si="2"/>
-        <v>6.6317226399270623E-6</v>
-      </c>
-      <c r="J7" s="15">
-        <f t="shared" si="0"/>
-        <v>2.4003711063098552E-6</v>
-      </c>
-      <c r="K7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" s="12">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L7" s="12">
-        <f t="shared" si="1"/>
-        <v>5.4262496754479805E-2</v>
-      </c>
-      <c r="M7" s="8">
+        <v>5.42626135753701E-2</v>
+      </c>
+      <c r="Q7" s="8">
         <f t="shared" si="4"/>
-        <v>3.4751668768961935E-2</v>
-      </c>
-      <c r="N7" s="8" t="b">
+        <v>3.4751746185270188E-2</v>
+      </c>
+      <c r="R7" s="8" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="17">
         <v>1.43328539923927</v>
@@ -1145,38 +3087,53 @@
         <v>4.6038332682662597</v>
       </c>
       <c r="G8" s="17">
-        <v>1.27394079067161</v>
+        <v>1.27394079066307</v>
       </c>
       <c r="H8" s="17">
         <v>3.3845987314102701</v>
       </c>
-      <c r="I8" s="18">
-        <f t="shared" si="2"/>
+      <c r="I8" s="17">
+        <v>0.84987047152756601</v>
+      </c>
+      <c r="J8" s="17">
+        <v>3.9127558368689099</v>
+      </c>
+      <c r="K8" s="17">
+        <v>1.3691704716730699</v>
+      </c>
+      <c r="L8" s="17">
+        <v>6.0701466343454697</v>
+      </c>
+      <c r="M8" s="18">
+        <f t="shared" si="1"/>
         <v>-4.2749583784339906E-2</v>
       </c>
-      <c r="J8" s="19">
+      <c r="N8" s="19">
         <f t="shared" si="0"/>
         <v>-2.9826288474737592E-2</v>
       </c>
-      <c r="K8" s="9" t="b">
+      <c r="O8" s="9" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P8" s="13">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L8" s="13">
-        <f t="shared" si="1"/>
         <v>-2.9653539499898685E-3</v>
       </c>
-      <c r="M8" s="9">
+      <c r="Q8" s="9">
         <f t="shared" si="4"/>
         <v>-6.4369081289758847E-4</v>
       </c>
-      <c r="N8" s="9" t="b">
+      <c r="R8" s="9" t="b">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="N2:N8 J2:K8">
+  <conditionalFormatting sqref="R2:R8 N2:O8">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -1184,25 +3141,26 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="M2:M8">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="notBetween">
       <formula>-0.1</formula>
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L8">
+  <conditionalFormatting sqref="P2:P8">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="notBetween">
       <formula>-0.1</formula>
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M8">
+  <conditionalFormatting sqref="Q2:Q8">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="notBetween">
       <formula>-0.1</formula>
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>